<commit_message>
[what] add sample input and output data
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juihungkao/blockchain-based-teais-js/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0E73B0F-6A0F-5243-81E9-A534154C7CFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F7B635E-E039-EA46-9602-E07F6950C05B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-2080" yWindow="-21600" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="AT_list" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="ref_table_companyA" sheetId="2" r:id="rId2"/>
     <sheet name="FS_companyA" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -919,7 +919,7 @@
   <dimension ref="A1:X31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>